<commit_message>
Updates to most roles
</commit_message>
<xml_diff>
--- a/Assets/Cards/Player Cards/Minister of Commerce.xlsx
+++ b/Assets/Cards/Player Cards/Minister of Commerce.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\keremataman\GitHub\kardashev-scale\Assets\Cards\Player Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE4B2D2-6D1B-4946-9C02-8344AB36993E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06669E51-7B5B-4B07-8B64-CAC28E04D9FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1320" yWindow="0" windowWidth="27480" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,88 +25,120 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
   <si>
     <t>Text</t>
   </si>
   <si>
-    <t>Gold</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
-    <t>You may move any amount of Gold between Players</t>
-  </si>
-  <si>
-    <t>When you play this card, place 6 Gold on it. This card stays on the field until there is no more Gold on it
-At the start of your turn, take 2 Gold from this card. If there is no Gold remaining on this card, shuffle it back to the minister of commerce's deck</t>
-  </si>
-  <si>
-    <t>When you play this card, place 8 Gold on it. This card stays on the field until there is no more Gold on it
-At the start of your turn, take 2 Gold from this card. If there is no Gold remaining on this card, shuffle it back to the minister of commerce's deck</t>
-  </si>
-  <si>
-    <t>When you play this card, place 12 Gold on it. This card stays on the field until there is no more Gold on it
-At the start of your turn, take 3 Gold from this card. If there is no Gold remaining on this card, shuffle it back to the minister of commerce's deck</t>
-  </si>
-  <si>
-    <t>When you play this card, place 16 Gold on it. This card stays on the field until there is no more Gold on it
-At the start of your turn, take 2 Gold from this card. If there is no Gold remaining on this card, shuffle it back to the minister of commerce's deck</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
+    <t>Investment</t>
+  </si>
+  <si>
+    <t>Stonks</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Push your luck</t>
+  </si>
+  <si>
+    <t>Derivatives</t>
+  </si>
+  <si>
+    <t>… And Taxes</t>
+  </si>
+  <si>
     <t>When you play this card, shuffle it into the event deck
-When this card is drawn from the event deck, each Player doubles their money. Then, shuffle this card into MoC's deck</t>
-  </si>
-  <si>
-    <t>Investment</t>
-  </si>
-  <si>
-    <t>Stonks</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Select a player, put this card in front of them, then put 2X Gold on this card. On their next turn, if they do a check and are successful, receive all the gold on this card. Otherwise, lose all gold on this card</t>
-  </si>
-  <si>
-    <t>Receive 3 Gold</t>
-  </si>
-  <si>
-    <t>Successful Speculation</t>
-  </si>
-  <si>
-    <t>Push your luck</t>
-  </si>
-  <si>
-    <t>Call Heads or Tails, then toss a coin. If successful, gain 2X gold</t>
-  </si>
-  <si>
-    <t>Pick a deck, put this card in front of it, then place 2X gold on this card. 
-Just before a card is drawn from that deck, guess the name of the card that will be drawn. If successful, receive all the Gold on this card. Otherwise, lose all the gold on this card</t>
-  </si>
-  <si>
-    <t>Pick a meter, guess which way it will go next, then put this card in the direction called and place 2X gold on this card. 
-When the meter moves, if it moves in the guessed direction, gain 2X gold. Otherwise, lose 2X gold</t>
-  </si>
-  <si>
-    <t>Call a number, then roll a die. If successful, gain 6X gold.</t>
-  </si>
-  <si>
-    <t>Derivatives</t>
-  </si>
-  <si>
-    <t>Place 4X gold on this card. If another "Stonks" card is successful until your next turn, gain all the gold on this card. Otherwise, lose all the gold on this card</t>
-  </si>
-  <si>
-    <t>… And Taxes</t>
-  </si>
-  <si>
-    <t>Gain 1 Gold for each Tile you own</t>
+When this card is played from the event deck, each Player doubles their money. Then, shuffle this card into MoC's deck</t>
+  </si>
+  <si>
+    <t>Hedge Funds</t>
+  </si>
+  <si>
+    <t>Credits</t>
+  </si>
+  <si>
+    <t>You may edit how much Credits at the end of the turn each player receives</t>
+  </si>
+  <si>
+    <t>When you play this card, place 6 Credits on it. This card stays on the field until there is no more Credits on it
+At the start of your turn, take 2 Credits from this card. If there is no Credits remaining on this card, shuffle it back to the minister of commerce's deck</t>
+  </si>
+  <si>
+    <t>When you play this card, place 8 Credits on it. This card stays on the field until there is no more Credits on it
+At the start of your turn, take 2 Credits from this card. If there is no Credits remaining on this card, shuffle it back to the minister of commerce's deck</t>
+  </si>
+  <si>
+    <t>When you play this card, place 12 Credits on it. This card stays on the field until there is no more Credits on it
+At the start of your turn, take 3 Credits from this card. If there is no Credits remaining on this card, shuffle it back to the minister of commerce's deck</t>
+  </si>
+  <si>
+    <t>When you play this card, place 16 Credits on it. This card stays on the field until there is no more Credits on it
+At the start of your turn, take 2 Credits from this card. If there is no Credits remaining on this card, shuffle it back to the minister of commerce's deck</t>
+  </si>
+  <si>
+    <t>Receive 3 Credits</t>
+  </si>
+  <si>
+    <t>Call Heads or Tails, then toss a coin. If successful, gain 2X Credits</t>
+  </si>
+  <si>
+    <t>Call a number, then roll a die. If successful, gain 6X Credits.</t>
+  </si>
+  <si>
+    <t>Gain 1 Credits for each Tile you own</t>
+  </si>
+  <si>
+    <t>Gain 9 Credits</t>
+  </si>
+  <si>
+    <t>Risk (get it?)</t>
+  </si>
+  <si>
+    <t>Place this card in front of Minister of Science. Until the end of next turn, whenever a successful research is made, gain credits equal to the tier of that research</t>
+  </si>
+  <si>
+    <t>Select a player, put this card in front of them, then put 2X Credits on this card. Until the end of this turn, if they do a check and are successful, receive all the Credits on this card.</t>
+  </si>
+  <si>
+    <t>Pick a meter, guess which way it will go next, then put this card in the direction called and place 2X Credits on this card. 
+When the meter moves, if it moves in the guessed direction, gain 2X Credits.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Place 4X Credits on this card. If another "Stonks" card is successful until end of the next turn, gain all the Credits on this card. </t>
+  </si>
+  <si>
+    <t>Place this card in front of the Minister of Defence. Until the end of this turn, whenever they successfully attack or defend a tile, gain Credits equal to the number of enemy Troops</t>
+  </si>
+  <si>
+    <t>Salt to the wound</t>
+  </si>
+  <si>
+    <t>Place this card in front of a Foreign Nation. Until the end of this turn, whenever a card that Foreign Nation plays gets negated, gain 3 Credits</t>
+  </si>
+  <si>
+    <t>YOLO</t>
+  </si>
+  <si>
+    <t>Place all your Credits on this card. Guess which resources the next World Event will affect. If you guess correctly, gain Credits equalling the Credits you put on this card times the number of successfully guessed resources</t>
+  </si>
+  <si>
+    <t>Place this card in front of Minister of Foreign Affaris. Until the end of the next turn, whenever a successful aggreement is made, gain 4 Credits</t>
+  </si>
+  <si>
+    <t>Trust</t>
+  </si>
+  <si>
+    <t>Science = Profit = Science</t>
+  </si>
+  <si>
+    <t>Diversification</t>
   </si>
 </sst>
 </file>
@@ -122,12 +154,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -142,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -150,6 +188,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,65 +490,68 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -517,104 +562,160 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" t="s">
-        <v>12</v>
+      <c r="B14">
+        <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>